<commit_message>
feat: Revert PSM caliper to 0.02 and re-run analysis
Changes:
- Updated psm_new_controls.py caliper from 0.01 to 0.02
- Re-ran PSM analysis: 2,846 obs matched (199 cities)
- Re-ran PSM-DID regression with new matched sample
- Updated CLAUDE.md with latest results
- Added .gitignore entry for nul file

PSM Results (caliper=0.02):
- Matched sample: 2,846 obs × 199 cities (increased from 2,648)
- Match rate: 91.3% average (better than caliper=0.01)
- All 5 covariates satisfy balance criterion (|bias| < 10%)

PSM-DID Results:
- Model 1 (no controls): DID coef = 0.0226 (p=0.434)
- Model 2 (with controls): DID coef = 0.0275 (p=0.329)
- Control variables: ln_pgdp***, industrial_advanced***, ln_road_area***
- Conclusion: Policy effect remains insignificant

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/人均GDP+人口集聚程度+产业高级化+外商投资水平+人均道路面积/PSM-DID基准回归结果表.xlsx
+++ b/人均GDP+人口集聚程度+产业高级化+外商投资水平+人均道路面积/PSM-DID基准回归结果表.xlsx
@@ -478,27 +478,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9.4477***</t>
+          <t>9.4695***</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.0319</t>
+          <t>0.0278</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14.4000***</t>
+          <t>14.3785***</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1.9335</t>
+          <t>1.9272</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>7.4476</t>
+          <t>7.4610</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -515,32 +515,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.0318</t>
+          <t>0.0226</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.0305</t>
+          <t>0.0288</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.0336</t>
+          <t>0.0275</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.0296</t>
+          <t>0.0282</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.1330</t>
+          <t>0.9761</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.2573</t>
+          <t>0.3291</t>
         </is>
       </c>
     </row>
@@ -554,22 +554,22 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-0.3925***</t>
+          <t>-0.3598***</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.1352</t>
+          <t>0.1333</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-2.9033</t>
+          <t>-2.6986</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.0037</t>
+          <t>0.0070</t>
         </is>
       </c>
     </row>
@@ -583,22 +583,22 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-0.2045</t>
+          <t>-0.2505</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.1688</t>
+          <t>0.1670</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-1.2119</t>
+          <t>-1.4999</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.2257</t>
+          <t>0.1337</t>
         </is>
       </c>
     </row>
@@ -612,22 +612,22 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-0.0827***</t>
+          <t>-0.0841***</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.0246</t>
+          <t>0.0243</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-3.3549</t>
+          <t>-3.4612</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.0008</t>
+          <t>0.0005</t>
         </is>
       </c>
     </row>
@@ -641,22 +641,22 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>-1.0973</t>
+          <t>-0.9608</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.7206</t>
+          <t>0.7121</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-1.5228</t>
+          <t>-1.3493</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.1279</t>
+          <t>0.1773</t>
         </is>
       </c>
     </row>
@@ -670,22 +670,22 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.1106**</t>
+          <t>0.1150***</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.0455</t>
+          <t>0.0445</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2.4311</t>
+          <t>2.5823</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.0151</t>
+          <t>0.0099</t>
         </is>
       </c>
     </row>
@@ -696,11 +696,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2648</v>
+        <v>2846</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>2648</v>
+        <v>2846</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -731,13 +731,13 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.9665</t>
+          <t>0.9677</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.9686</t>
+          <t>0.9697</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -752,13 +752,13 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.9635</t>
+          <t>0.9651</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.9657</t>
+          <t>0.9671</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>

</xml_diff>